<commit_message>
criação de views, joins etc
</commit_message>
<xml_diff>
--- a/test/output.xlsx
+++ b/test/output.xlsx
@@ -7,8 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="N100 - Listagem NFe" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="N170 - Itens NFe" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="0200 - Produtos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="0150 - Participantes" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="C100 - E_S" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -430,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,170 +442,56 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>N100</t>
+          <t>COD_ITEM</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>CNPJ_EMIT</t>
+          <t>DESCR_ITEM</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>NOME_EMIT</t>
+          <t>COD_NCM</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>NUM_NFE</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>SERIE</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>DT_EMISSAO</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>TIPO_NFE</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>CHAVE_NFE</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>CNPJ_DEST</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>CPF_DEST</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>NOME_DEST</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>UF</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>VALOR_NFE</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr"/>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>MES_ANO</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>DATA_IMPORTACAO</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>STATUS_NFE</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>X_USER1</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>X_USER2</t>
+          <t>CEST</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>N100</t>
+          <t>DESP00191</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>23004906000180</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>TESTE LTDA</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>135418</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>45414</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>SAIDA</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>35240523004906000180550010001354181002078142</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>23.004.906/0001-80</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>DANIELA EVANGELISTA DA SILVA</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>BA</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>80</v>
-      </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>05_2024</t>
-        </is>
-      </c>
-      <c r="P2" s="2" t="n">
-        <v>45562</v>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>AUTORIZADA</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
+          <t>BIODIGESTOR 700L - FORTLEV</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>78985640447416</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>QI10WG CARREGADOR DE INDUCAO PARA APARELHOS CELULARES COM 5W NF Ent: 00054862F1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>85044010</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -617,7 +504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,293 +515,518 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>N100</t>
+          <t>COD_PART</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>CNPJ_EMIT</t>
+          <t>NOME</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>NUM_NFE</t>
+          <t>COD_PAIS</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>SERIE</t>
+          <t>CNPJ</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>N170</t>
+          <t>CPF</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>CNPJ_EMIT</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>NUM_NFE</t>
+          <t>COD_MUN</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>SERIE</t>
+          <t>SUFRAMA</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>NUM_ITEM</t>
+          <t>END</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>COD_PROD</t>
+          <t>NUM</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>DESC_PROD</t>
+          <t>COMPL</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>NCM</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>CFOP</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>VLR_UNIT</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>QTDE</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>UNID</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>VLR_PROD</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>VLR_FRETE</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>VLR_SEGURO</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>VLR_DESC</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>VLR_OUTROS</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>VLR_ITEM</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>ORIGEM</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>CST_ICMS</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>BC_ICMS</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>ALQ_ICMS</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>VLR_ICMS</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>MVA</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>BC_ICMSST</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>ALQ_ICMSST</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>ICMSST</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>CST_IPI</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>VLR_IPI</t>
+          <t>BAIRRO</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>N100</t>
+          <t>CLI000000503</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>23004906000180</t>
+          <t>CONSTRUTONI MATERIAIS PARA CON</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>135418</t>
+          <t>1058</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>05923344000196</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>7012595100085</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>3170107</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>AVENIDA ORLANDO RODRIGUES DA CUNHA</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>VL SAO VICENTE</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FOR000028800</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TRANSPORTADORA Y23 EIRELI</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1058</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>39848198000101</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0039007510061</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>3125101</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>RUA ANTONIO MOREIRA FILHO</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>DOS TENENTES</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FOR000030040</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PELOG ARMAZENS GERAIS LTDA.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>01058</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>03986934000132</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>206644676115</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>3505708</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>AVENIDA MARCOS PENTEADO DE ULHOA RODRIGU</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>491</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>TAMBORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FOR000026707</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>EFIZI AZU COMERCIO LTDA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1058</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>34229157000105</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>083582452</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>3205002</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>RUA 7 A</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>SETOR B SALA 1</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>CIVIT II</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>C100.IND_OPER</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>C100.IND_EMIT</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>C100.COD_PART</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>C100.COD_MOD</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>C100.COD_SIT</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>C100.SER</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>C100.NUM_DOC</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>C100.DT_DOC</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>C100.VL_DOC</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>NUM_ITEM</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>COD_ITEM</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>0200.COD_NCM</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>QTD</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>UNID</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>VL_ITEM</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>CFOP</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>CST_ICMS</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>VL_BC_ICMS</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>ALIQ_ICMS</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>VL_ICMS</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>VL_BC_ICMS_ST</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>VL_ICMS_ST</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>VL_IPI</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>FOR000030040</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>N170</t>
+          <t>00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>23004906000180</t>
+          <t>004</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>135418</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
+          <t>78662</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>45415</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>561.80</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>AERCX02RD</t>
-        </is>
-      </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>CAIXA DE SOM BLUETOOTH COR VERMELHO CARMIM AERBOX 2</t>
+          <t>78985640447416</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>85182100</t>
+          <t>85044010</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2949</t>
-        </is>
-      </c>
-      <c r="N2" t="n">
-        <v>80</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1</v>
+          <t>20.0000</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>561.80</t>
+        </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="Q2" t="n">
-        <v>80</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>80</v>
-      </c>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="n">
-        <v>80</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
-      </c>
-      <c r="AG2" t="n">
-        <v>0</v>
+          <t>1907</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>141</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>